<commit_message>
Improved CHR sudoku solver
</commit_message>
<xml_diff>
--- a/sudoku/Benchmarks.xlsx
+++ b/sudoku/Benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Universiteit\Semester 8\APLAI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unief\APLAI\Git Project\APLAI\sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA304AF-96F4-4DA3-A586-4553477E7F29}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E5B7AD-6840-447F-9E2D-CA5D0184EA35}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{4EEA1ADA-0D90-41F2-BA1B-48004A46E488}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="9" xr2:uid="{4EEA1ADA-0D90-41F2-BA1B-48004A46E488}"/>
   </bookViews>
   <sheets>
     <sheet name="IOGlobal" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="CHR_New" sheetId="11" r:id="rId11"/>
     <sheet name="CHR_Both" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -123,6 +122,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,10 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -3571,46 +3574,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>117.68900000000001</c:v>
+                  <c:v>9.9220000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.968333333333334</c:v>
+                  <c:v>2.6406666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0936666666666666</c:v>
+                  <c:v>1.0780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.296333333333331</c:v>
+                  <c:v>1.5523333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.989000000000004</c:v>
+                  <c:v>2.5779999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.346666666666664</c:v>
+                  <c:v>7.5676666666666668</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.164333333333332</c:v>
+                  <c:v>8.0990000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>122.05333333333333</c:v>
+                  <c:v>11.396000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>296.58833333333337</c:v>
+                  <c:v>28.145666666666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3906666666666667</c:v>
+                  <c:v>0.70333333333333325</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55.029333333333334</c:v>
+                  <c:v>5.7033333333333331</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>118.64700000000001</c:v>
+                  <c:v>11.317666666666668</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>74.284000000000006</c:v>
+                  <c:v>8.0366666666666671</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.06133333333333</c:v>
+                  <c:v>3.3126666666666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3694,46 +3697,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1685.443</c:v>
+                  <c:v>0.48966666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.53633333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.058999999999997</c:v>
+                  <c:v>0.505</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9529999999999998</c:v>
+                  <c:v>1.9793333333333336</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>432.61</c:v>
+                  <c:v>1.7916666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>166.35400000000001</c:v>
+                  <c:v>0.45833333333333331</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.3126666666666669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.52100000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.53133333333333344</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>148.245</c:v>
+                  <c:v>10.432</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.73433333333333328</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.55766666666666664</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1481.1010000000001</c:v>
+                  <c:v>0.42133333333333334</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>209.24299999999999</c:v>
+                  <c:v>0.8696666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3817,46 +3820,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>196.39933333333332</c:v>
+                  <c:v>10.352333333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.227666666666664</c:v>
+                  <c:v>3.0626666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.843333333333334</c:v>
+                  <c:v>1.2969999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.817333333333334</c:v>
+                  <c:v>1.6719999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.961999999999996</c:v>
+                  <c:v>2.5363333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118.85166666666667</c:v>
+                  <c:v>6.8959999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120.267</c:v>
+                  <c:v>7.5303333333333322</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>195.49333333333334</c:v>
+                  <c:v>10.151333333333334</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>484.041</c:v>
+                  <c:v>24.640666666666664</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.3280000000000003</c:v>
+                  <c:v>0.94299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.64800000000001</c:v>
+                  <c:v>5.2603333333333326</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>183.21766666666667</c:v>
+                  <c:v>9.9846666666666675</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120.22533333333332</c:v>
+                  <c:v>7.6196666666666664</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>63.524000000000001</c:v>
+                  <c:v>3.7029999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4340,49 +4343,49 @@
             <c:numRef>
               <c:f>CHR_Classic!$F$2:$F$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>951909636</c:v>
+                  <c:v>77497072</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>219401287</c:v>
+                  <c:v>19688716</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55968026</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="#,##0">
-                  <c:v>89804687</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="#,##0">
-                  <c:v>185983068</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
-                  <c:v>601439956</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
-                  <c:v>585693705</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
-                  <c:v>951909631</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
-                  <c:v>2390048510</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>18201825</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
-                  <c:v>441908843</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="#,##0">
-                  <c:v>932278773</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="#,##0">
-                  <c:v>596205502</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="#,##0">
-                  <c:v>292096875</c:v>
+                  <c:v>9223416</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14296191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25584971</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78875129</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82495849</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>118499691</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>302845877</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4706694</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58491747</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>118108562</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>83464818</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26313898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4463,31 +4466,49 @@
             <c:numRef>
               <c:f>CHR_New!$F$2:$F$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="#,##0">
-                  <c:v>13210174211</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="#,##0">
-                  <c:v>728673522</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="#,##0">
-                  <c:v>30211084</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="#,##0">
-                  <c:v>3435991885</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
-                  <c:v>1280248534</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>1137887589</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="#,##0">
-                  <c:v>11052838146</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="#,##0">
-                  <c:v>1616165240</c:v>
+                <c:pt idx="0">
+                  <c:v>2480101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2495013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2558857</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16913563</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15252365</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2514390</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19487520</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2480101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2618827</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99931403</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4633754</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2581245</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2188590</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6546132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4571,46 +4592,46 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1609591558</c:v>
+                  <c:v>83962721</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>351973747</c:v>
+                  <c:v>21917673</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92340460</c:v>
+                  <c:v>7094581</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>148789340</c:v>
+                  <c:v>10575208</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>302128115</c:v>
+                  <c:v>18791459</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>964447287</c:v>
+                  <c:v>56178110</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>970717911</c:v>
+                  <c:v>59317466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1609591956</c:v>
+                  <c:v>83962721</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3979902894</c:v>
+                  <c:v>212577280</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30016108</c:v>
+                  <c:v>3989545</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>728346627</c:v>
+                  <c:v>41297622</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1522669463</c:v>
+                  <c:v>83615377</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>987779799</c:v>
+                  <c:v>60546505</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>483028805</c:v>
+                  <c:v>28606253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4825,7 +4846,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -9062,8 +9083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE63E4D5-603C-4D1F-9F47-80261D74981C}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9099,20 +9120,20 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>117.387</v>
+        <v>9.9060000000000006</v>
       </c>
       <c r="C2">
-        <v>118.512</v>
+        <v>9.9380000000000006</v>
       </c>
       <c r="D2">
-        <v>117.16800000000001</v>
+        <v>9.9220000000000006</v>
       </c>
       <c r="E2">
         <f>AVERAGE(B2:D2)</f>
-        <v>117.68900000000001</v>
-      </c>
-      <c r="F2">
-        <v>951909636</v>
+        <v>9.9220000000000006</v>
+      </c>
+      <c r="F2" s="2">
+        <v>77497072</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9120,20 +9141,20 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>28.093</v>
+        <v>2.609</v>
       </c>
       <c r="C3">
-        <v>27.748999999999999</v>
+        <v>2.6720000000000002</v>
       </c>
       <c r="D3">
-        <v>28.062999999999999</v>
+        <v>2.641</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E15" si="0">AVERAGE(B3:D3)</f>
-        <v>27.968333333333334</v>
-      </c>
-      <c r="F3">
-        <v>219401287</v>
+        <v>2.6406666666666667</v>
+      </c>
+      <c r="F3" s="2">
+        <v>19688716</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9141,20 +9162,20 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>7.0469999999999997</v>
+        <v>1.0780000000000001</v>
       </c>
       <c r="C4">
-        <v>7.109</v>
+        <v>1.0780000000000001</v>
       </c>
       <c r="D4">
-        <v>7.125</v>
+        <v>1.0780000000000001</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>7.0936666666666666</v>
-      </c>
-      <c r="F4">
-        <v>55968026</v>
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>9223416</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9162,20 +9183,20 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>11.311999999999999</v>
+        <v>1.5469999999999999</v>
       </c>
       <c r="C5">
-        <v>11.281000000000001</v>
+        <v>1.5469999999999999</v>
       </c>
       <c r="D5">
-        <v>11.295999999999999</v>
+        <v>1.5629999999999999</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>11.296333333333331</v>
+        <v>1.5523333333333333</v>
       </c>
       <c r="F5" s="2">
-        <v>89804687</v>
+        <v>14296191</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9183,20 +9204,20 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>23.295999999999999</v>
+        <v>2.5310000000000001</v>
       </c>
       <c r="C6">
-        <v>22.937000000000001</v>
+        <v>2.5939999999999999</v>
       </c>
       <c r="D6">
-        <v>22.734000000000002</v>
+        <v>2.609</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>22.989000000000004</v>
+        <v>2.5779999999999998</v>
       </c>
       <c r="F6" s="2">
-        <v>185983068</v>
+        <v>25584971</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -9204,20 +9225,20 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>74.248000000000005</v>
+        <v>7.5309999999999997</v>
       </c>
       <c r="C7">
-        <v>74.06</v>
+        <v>7.5940000000000003</v>
       </c>
       <c r="D7">
-        <v>74.731999999999999</v>
+        <v>7.5780000000000003</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>74.346666666666664</v>
+        <v>7.5676666666666668</v>
       </c>
       <c r="F7" s="2">
-        <v>601439956</v>
+        <v>78875129</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9225,20 +9246,20 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>72.123000000000005</v>
+        <v>8.109</v>
       </c>
       <c r="C8">
-        <v>72.153999999999996</v>
+        <v>8.0630000000000006</v>
       </c>
       <c r="D8">
-        <v>72.215999999999994</v>
+        <v>8.125</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>72.164333333333332</v>
+        <v>8.0990000000000002</v>
       </c>
       <c r="F8" s="2">
-        <v>585693705</v>
+        <v>82495849</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9246,20 +9267,20 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>121.496</v>
+        <v>11.391</v>
       </c>
       <c r="C9">
-        <v>128.10499999999999</v>
+        <v>11.406000000000001</v>
       </c>
       <c r="D9">
-        <v>116.559</v>
+        <v>11.391</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>122.05333333333333</v>
+        <v>11.396000000000001</v>
       </c>
       <c r="F9" s="2">
-        <v>951909631</v>
+        <v>118499691</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9267,20 +9288,20 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>304.113</v>
+        <v>28.109000000000002</v>
       </c>
       <c r="C10">
-        <v>292.94299999999998</v>
+        <v>28.155999999999999</v>
       </c>
       <c r="D10">
-        <v>292.709</v>
+        <v>28.172000000000001</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>296.58833333333337</v>
+        <v>28.145666666666667</v>
       </c>
       <c r="F10" s="2">
-        <v>2390048510</v>
+        <v>302845877</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -9288,20 +9309,20 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>2.375</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="C11">
-        <v>2.375</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="D11">
-        <v>2.4220000000000002</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>2.3906666666666667</v>
+        <v>0.70333333333333325</v>
       </c>
       <c r="F11" s="2">
-        <v>18201825</v>
+        <v>4706694</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9309,20 +9330,20 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>54.514000000000003</v>
+        <v>5.7190000000000003</v>
       </c>
       <c r="C12">
-        <v>54.795000000000002</v>
+        <v>5.7190000000000003</v>
       </c>
       <c r="D12">
-        <v>55.779000000000003</v>
+        <v>5.6719999999999997</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>55.029333333333334</v>
+        <v>5.7033333333333331</v>
       </c>
       <c r="F12" s="2">
-        <v>441908843</v>
+        <v>58491747</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9330,20 +9351,20 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>127.23</v>
+        <v>11.327999999999999</v>
       </c>
       <c r="C13">
-        <v>114.512</v>
+        <v>11.327999999999999</v>
       </c>
       <c r="D13">
-        <v>114.199</v>
+        <v>11.297000000000001</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>118.64700000000001</v>
+        <v>11.317666666666668</v>
       </c>
       <c r="F13" s="2">
-        <v>932278773</v>
+        <v>118108562</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9351,20 +9372,20 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>75.465999999999994</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>73.56</v>
+        <v>8.0470000000000006</v>
       </c>
       <c r="D14">
-        <v>73.825999999999993</v>
+        <v>8.0630000000000006</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>74.284000000000006</v>
+        <v>8.0366666666666671</v>
       </c>
       <c r="F14" s="2">
-        <v>596205502</v>
+        <v>83464818</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9372,20 +9393,20 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>36.311</v>
+        <v>3.3130000000000002</v>
       </c>
       <c r="C15">
-        <v>35.874000000000002</v>
+        <v>3.2970000000000002</v>
       </c>
       <c r="D15">
-        <v>35.999000000000002</v>
+        <v>3.3279999999999998</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>36.06133333333333</v>
+        <v>3.3126666666666669</v>
       </c>
       <c r="F15" s="2">
-        <v>292096875</v>
+        <v>26313898</v>
       </c>
     </row>
   </sheetData>
@@ -9398,7 +9419,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="A1:F15"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9433,23 +9454,41 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1685.443</v>
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.46899999999999997</v>
       </c>
       <c r="E2">
         <f>AVERAGE(B2:D2)</f>
-        <v>1685.443</v>
+        <v>0.48966666666666664</v>
       </c>
       <c r="F2" s="2">
-        <v>13210174211</v>
+        <v>2480101</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="e">
+      <c r="B3">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="C3">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="E3">
         <f t="shared" ref="E3:E15" si="0">AVERAGE(B3:D3)</f>
-        <v>#DIV/0!</v>
+        <v>0.53633333333333333</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2495013</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9457,14 +9496,20 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>92.058999999999997</v>
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="D4">
+        <v>0.48399999999999999</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>92.058999999999997</v>
+        <v>0.505</v>
       </c>
       <c r="F4" s="2">
-        <v>728673522</v>
+        <v>2558857</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9472,14 +9517,20 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>3.9529999999999998</v>
+        <v>1.9530000000000001</v>
+      </c>
+      <c r="C5">
+        <v>1.9690000000000001</v>
+      </c>
+      <c r="D5">
+        <v>2.016</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>3.9529999999999998</v>
+        <v>1.9793333333333336</v>
       </c>
       <c r="F5" s="2">
-        <v>30211084</v>
+        <v>16913563</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9487,14 +9538,20 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>432.61</v>
+        <v>1.75</v>
+      </c>
+      <c r="C6">
+        <v>1.7969999999999999</v>
+      </c>
+      <c r="D6">
+        <v>1.8280000000000001</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>432.61</v>
+        <v>1.7916666666666667</v>
       </c>
       <c r="F6" s="2">
-        <v>3435991885</v>
+        <v>15252365</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -9502,94 +9559,167 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>166.35400000000001</v>
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.46899999999999997</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>166.35400000000001</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="F7" s="2">
-        <v>1280248534</v>
+        <v>2514390</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="B8" s="3">
+        <v>2.2970000000000002</v>
+      </c>
+      <c r="C8">
+        <v>2.3279999999999998</v>
+      </c>
+      <c r="D8">
+        <v>2.3130000000000002</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2.3126666666666669</v>
+      </c>
+      <c r="F8" s="2">
+        <v>19487520</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="2"/>
+      <c r="B9">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="D9">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2480101</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="2"/>
+      <c r="B10">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D10">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.53133333333333344</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2618827</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>148.245</v>
+        <v>10.406000000000001</v>
+      </c>
+      <c r="C11">
+        <v>10.436999999999999</v>
+      </c>
+      <c r="D11">
+        <v>10.452999999999999</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>148.245</v>
+        <v>10.432</v>
       </c>
       <c r="F11" s="2">
-        <v>1137887589</v>
+        <v>99931403</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" s="2"/>
+      <c r="B12">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="C12">
+        <v>0.75</v>
+      </c>
+      <c r="D12">
+        <v>0.75</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.73433333333333328</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4633754</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="2"/>
+      <c r="B13">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="C13">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="D13">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.55766666666666664</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2581245</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>1481.1010000000001</v>
+        <v>0.42</v>
+      </c>
+      <c r="C14">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="D14">
+        <v>0.438</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>1481.1010000000001</v>
+        <v>0.42133333333333334</v>
       </c>
       <c r="F14" s="2">
-        <v>11052838146</v>
+        <v>2188590</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9597,14 +9727,20 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>209.24299999999999</v>
+        <v>0.875</v>
+      </c>
+      <c r="C15">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.875</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>209.24299999999999</v>
+        <v>0.8696666666666667</v>
       </c>
       <c r="F15" s="2">
-        <v>1616165240</v>
+        <v>6546132</v>
       </c>
     </row>
   </sheetData>
@@ -9617,7 +9753,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9650,20 +9786,20 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>193.49299999999999</v>
+        <v>10.231999999999999</v>
       </c>
       <c r="C2">
-        <v>201.99299999999999</v>
+        <v>10.609</v>
       </c>
       <c r="D2">
-        <v>193.71199999999999</v>
+        <v>10.215999999999999</v>
       </c>
       <c r="E2">
         <f>AVERAGE(B2:D2)</f>
-        <v>196.39933333333332</v>
+        <v>10.352333333333334</v>
       </c>
       <c r="F2" s="2">
-        <v>1609591558</v>
+        <v>83962721</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9671,20 +9807,20 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>43.311</v>
+        <v>3.0939999999999999</v>
       </c>
       <c r="C3">
-        <v>42.764000000000003</v>
+        <v>3.0630000000000002</v>
       </c>
       <c r="D3">
-        <v>43.607999999999997</v>
+        <v>3.0310000000000001</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E15" si="0">AVERAGE(B3:D3)</f>
-        <v>43.227666666666664</v>
+        <v>3.0626666666666669</v>
       </c>
       <c r="F3" s="2">
-        <v>351973747</v>
+        <v>21917673</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9692,20 +9828,20 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>11.781000000000001</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="C4">
-        <v>11.843</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="D4">
-        <v>11.906000000000001</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>11.843333333333334</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="F4" s="2">
-        <v>92340460</v>
+        <v>7094581</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9713,20 +9849,20 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>18.577999999999999</v>
+        <v>1.6719999999999999</v>
       </c>
       <c r="C5">
-        <v>18.859000000000002</v>
+        <v>1.6719999999999999</v>
       </c>
       <c r="D5">
-        <v>19.015000000000001</v>
+        <v>1.6719999999999999</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>18.817333333333334</v>
+        <v>1.6719999999999999</v>
       </c>
       <c r="F5" s="2">
-        <v>148789340</v>
+        <v>10575208</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9734,20 +9870,20 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>36.732999999999997</v>
+        <v>2.5939999999999999</v>
       </c>
       <c r="C6">
-        <v>37.389000000000003</v>
+        <v>2.4529999999999998</v>
       </c>
       <c r="D6">
-        <v>36.764000000000003</v>
+        <v>2.5619999999999998</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>36.961999999999996</v>
+        <v>2.5363333333333333</v>
       </c>
       <c r="F6" s="2">
-        <v>302128115</v>
+        <v>18791459</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -9755,20 +9891,20 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>116.09</v>
+        <v>6.859</v>
       </c>
       <c r="C7">
-        <v>116</v>
+        <v>6.891</v>
       </c>
       <c r="D7">
-        <v>124.465</v>
+        <v>6.9379999999999997</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>118.85166666666667</v>
+        <v>6.8959999999999999</v>
       </c>
       <c r="F7" s="2">
-        <v>964447287</v>
+        <v>56178110</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9776,20 +9912,20 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>124.777</v>
+        <v>7.5</v>
       </c>
       <c r="C8">
-        <v>118.387</v>
+        <v>7.5309999999999997</v>
       </c>
       <c r="D8">
-        <v>117.637</v>
+        <v>7.56</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>120.267</v>
+        <v>7.5303333333333322</v>
       </c>
       <c r="F8" s="2">
-        <v>970717911</v>
+        <v>59317466</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9797,20 +9933,20 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>193.66499999999999</v>
+        <v>10.141</v>
       </c>
       <c r="C9">
-        <v>195.54</v>
+        <v>10.141</v>
       </c>
       <c r="D9">
-        <v>197.27500000000001</v>
+        <v>10.172000000000001</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>195.49333333333334</v>
+        <v>10.151333333333334</v>
       </c>
       <c r="F9" s="2">
-        <v>1609591956</v>
+        <v>83962721</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9818,20 +9954,20 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>495.29599999999999</v>
+        <v>24.547000000000001</v>
       </c>
       <c r="C10">
-        <v>476.57799999999997</v>
+        <v>24.687000000000001</v>
       </c>
       <c r="D10">
-        <v>480.24900000000002</v>
+        <v>24.687999999999999</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>484.041</v>
+        <v>24.640666666666664</v>
       </c>
       <c r="F10" s="2">
-        <v>3979902894</v>
+        <v>212577280</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -9839,20 +9975,20 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>4.375</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="C11">
-        <v>4.25</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="D11">
-        <v>4.359</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>4.3280000000000003</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="F11" s="2">
-        <v>30016108</v>
+        <v>3989545</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9860,20 +9996,20 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>87.965999999999994</v>
+        <v>5.234</v>
       </c>
       <c r="C12">
-        <v>88.403000000000006</v>
+        <v>5.25</v>
       </c>
       <c r="D12">
-        <v>89.575000000000003</v>
+        <v>5.2969999999999997</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>88.64800000000001</v>
+        <v>5.2603333333333326</v>
       </c>
       <c r="F12" s="2">
-        <v>728346627</v>
+        <v>41297622</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9881,20 +10017,20 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>183.791</v>
+        <v>10.016</v>
       </c>
       <c r="C13">
-        <v>182.88399999999999</v>
+        <v>9.9689999999999994</v>
       </c>
       <c r="D13">
-        <v>182.97800000000001</v>
+        <v>9.9689999999999994</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>183.21766666666667</v>
+        <v>9.9846666666666675</v>
       </c>
       <c r="F13" s="2">
-        <v>1522669463</v>
+        <v>83615377</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9902,20 +10038,20 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>119.215</v>
+        <v>7.859</v>
       </c>
       <c r="C14">
-        <v>120.949</v>
+        <v>7.4690000000000003</v>
       </c>
       <c r="D14">
-        <v>120.512</v>
+        <v>7.5309999999999997</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>120.22533333333332</v>
+        <v>7.6196666666666664</v>
       </c>
       <c r="F14" s="2">
-        <v>987779799</v>
+        <v>60546505</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9923,20 +10059,20 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>60.466999999999999</v>
+        <v>3.7029999999999998</v>
       </c>
       <c r="C15">
-        <v>61.06</v>
+        <v>3.7189999999999999</v>
       </c>
       <c r="D15">
-        <v>69.045000000000002</v>
+        <v>3.6869999999999998</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>63.524000000000001</v>
+        <v>3.7029999999999998</v>
       </c>
       <c r="F15" s="2">
-        <v>483028805</v>
+        <v>28606253</v>
       </c>
     </row>
   </sheetData>
@@ -10948,7 +11084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802995EE-F77C-453E-B7D8-A767D82682F8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>

</xml_diff>